<commit_message>
Reiter und Text zugefügt
</commit_message>
<xml_diff>
--- a/SuperGitTestFile.xlsx
+++ b/SuperGitTestFile.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21480" windowHeight="12015"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Buch" sheetId="2" r:id="rId1"/>
+    <sheet name="Film" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,6 +22,26 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>Film</t>
+  </si>
+  <si>
+    <t>Buch1</t>
+  </si>
+  <si>
+    <t>Buch2</t>
+  </si>
+  <si>
+    <t>Seite</t>
+  </si>
+  <si>
+    <t>Datum</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -336,12 +357,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>